<commit_message>
Added sine-moving virus (v1.2.0)
</commit_message>
<xml_diff>
--- a/res/maps/level_1.xlsx
+++ b/res/maps/level_1.xlsx
@@ -227,7 +227,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,6 +254,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA64D79"/>
+        <bgColor rgb="FFA64D79"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FFFF0000"/>
       </patternFill>
@@ -262,6 +268,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
         <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9900FF"/>
+        <bgColor rgb="FF9900FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -271,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -291,6 +303,12 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -560,7 +578,7 @@
       <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -571,7 +589,7 @@
       <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -603,7 +621,7 @@
       <c r="D4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>28</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -620,7 +638,7 @@
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>33</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -661,7 +679,7 @@
       <c r="F6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="8" t="s">
         <v>46</v>
       </c>
       <c r="H6" s="2" t="s">

</xml_diff>